<commit_message>
update results and data
</commit_message>
<xml_diff>
--- a/results/results_4_tz1_transfer_learning_subsets_domain_importance.xlsx
+++ b/results/results_4_tz1_transfer_learning_subsets_domain_importance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TM\Dropbox\DS\RNN-for-TS\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30E0E86-D3ED-49FF-9DA4-66B57E7BCAE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C51CF86-DF10-488B-809B-0B442B086B1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="19200" windowHeight="10200" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="19200" windowHeight="10200" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m4_m_industry" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="m4_m_demographic" sheetId="3" r:id="rId3"/>
     <sheet name="m4_m_micro" sheetId="5" r:id="rId4"/>
     <sheet name="m4_q_macro" sheetId="4" r:id="rId5"/>
+    <sheet name="m4_q_micro" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="38">
   <si>
     <t>Method</t>
   </si>
@@ -146,6 +147,9 @@
   </si>
   <si>
     <t>True</t>
+  </si>
+  <si>
+    <t>m4_quarterly_micro</t>
   </si>
 </sst>
 </file>
@@ -4222,7 +4226,7 @@
   <dimension ref="A1:P91"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -6046,9 +6050,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5251949F-02FF-4061-ADE5-389DA13746F2}">
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I72" sqref="I72"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6114,6 +6118,12 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>48000</v>
+      </c>
+      <c r="B8">
+        <v>5728</v>
+      </c>
       <c r="E8" s="2">
         <v>1.6410450000000001</v>
       </c>
@@ -7232,7 +7242,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E49" s="2">
         <v>1.006246</v>
       </c>
@@ -7264,42 +7274,42 @@
         <v>31</v>
       </c>
     </row>
-    <row r="50" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="5:14" x14ac:dyDescent="0.35">
       <c r="J50">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="5:14" x14ac:dyDescent="0.35">
       <c r="J51">
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="5:14" x14ac:dyDescent="0.35">
       <c r="J52">
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="5:14" x14ac:dyDescent="0.35">
       <c r="J53">
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="5:14" x14ac:dyDescent="0.35">
       <c r="J54">
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="5:14" x14ac:dyDescent="0.35">
       <c r="J55">
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="5:14" x14ac:dyDescent="0.35">
       <c r="J56">
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E57" s="8">
         <f>AVERAGE(E47:E56)</f>
         <v>1.0998903333333334</v>
@@ -7313,7 +7323,7 @@
         <v>10.492464333333333</v>
       </c>
     </row>
-    <row r="58" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E58" s="8">
         <f>MEDIAN(E47:E56)</f>
         <v>1.054049</v>
@@ -7327,10 +7337,7 @@
         <v>9.9368119999999998</v>
       </c>
     </row>
-    <row r="60" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D60">
-        <v>0</v>
-      </c>
+    <row r="60" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E60">
         <v>1.5723750000000001</v>
       </c>
@@ -7362,10 +7369,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D61">
-        <v>0</v>
-      </c>
+    <row r="61" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E61">
         <v>1.581993</v>
       </c>
@@ -7397,10 +7401,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D62">
-        <v>0</v>
-      </c>
+    <row r="62" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E62">
         <v>1.0283800000000001</v>
       </c>
@@ -7432,12 +7433,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="5:14" x14ac:dyDescent="0.35">
       <c r="J63">
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="5:14" x14ac:dyDescent="0.35">
       <c r="J64">
         <v>46</v>
       </c>
@@ -8737,10 +8738,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF05622A-CE2B-42B3-9C4D-A6A11FE84B96}">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:P110"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8752,7 +8754,7 @@
     <col min="10" max="10" width="4.7265625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.7265625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.54296875" customWidth="1"/>
-    <col min="13" max="13" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.453125" customWidth="1"/>
     <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8807,19 +8809,28 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E8">
+      <c r="A8">
+        <v>24000</v>
+      </c>
+      <c r="B8">
+        <v>5315</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="2">
         <v>1.3166</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>0.102285</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>19.585228000000001</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="2">
         <v>9.5675999999999997E-2</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="2">
         <v>5.6813000000000002E-2</v>
       </c>
       <c r="J8">
@@ -8839,19 +8850,19 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E9">
+      <c r="E9" s="2">
         <v>1.4229259999999999</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>0.105006</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>18.330622999999999</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="2">
         <v>9.7353999999999996E-2</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="2">
         <v>5.7176999999999999E-2</v>
       </c>
       <c r="J9">
@@ -8871,19 +8882,19 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E10">
+      <c r="E10" s="2">
         <v>1.418569</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>0.105916</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>18.468132000000001</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="2">
         <v>9.7355999999999998E-2</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="2">
         <v>5.6090000000000001E-2</v>
       </c>
       <c r="J10">
@@ -8903,19 +8914,19 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E11">
+      <c r="E11" s="2">
         <v>1.364028</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>0.10267900000000001</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>20.238495</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <v>9.4742000000000007E-2</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="2">
         <v>5.9582999999999997E-2</v>
       </c>
       <c r="J11">
@@ -8935,19 +8946,19 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E12">
+      <c r="E12" s="2">
         <v>1.3637790000000001</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>0.103661</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>18.049384</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="2">
         <v>9.4943E-2</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="2">
         <v>5.7211999999999999E-2</v>
       </c>
       <c r="J12">
@@ -8967,19 +8978,19 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E13">
+      <c r="E13" s="2">
         <v>1.294381</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>0.101661</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>18.008749000000002</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="2">
         <v>9.4775999999999999E-2</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="2">
         <v>5.6987999999999997E-2</v>
       </c>
       <c r="J13">
@@ -8999,19 +9010,19 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E14">
+      <c r="E14" s="2">
         <v>1.9521580000000001</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>0.12199</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="2">
         <v>20.502330000000001</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="2">
         <v>0.109546</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="2">
         <v>5.9048999999999997E-2</v>
       </c>
       <c r="J14">
@@ -9031,19 +9042,19 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E15">
+      <c r="E15" s="2">
         <v>1.3103910000000001</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>0.102229</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="2">
         <v>17.624884000000002</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="2">
         <v>9.3329999999999996E-2</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="2">
         <v>5.7695999999999997E-2</v>
       </c>
       <c r="J15">
@@ -9063,19 +9074,19 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E16">
+      <c r="E16" s="2">
         <v>1.344047</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>0.102716</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="2">
         <v>19.315428000000001</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="2">
         <v>9.5077999999999996E-2</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="2">
         <v>5.8417999999999998E-2</v>
       </c>
       <c r="J16">
@@ -9094,20 +9105,20 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="E17">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E17" s="2">
         <v>1.369696</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>0.103271</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="2">
         <v>17.886839999999999</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="2">
         <v>9.7011E-2</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="2">
         <v>5.6633999999999997E-2</v>
       </c>
       <c r="J17">
@@ -9126,53 +9137,3343 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="5:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E18" s="8">
+        <f>AVERAGE(E8:E17)</f>
+        <v>1.4156574999999998</v>
+      </c>
+      <c r="F18" s="8">
+        <f>AVERAGE(F8:F17)</f>
+        <v>0.10514140000000001</v>
+      </c>
+      <c r="G18" s="8">
+        <f>AVERAGE(G8:G17)</f>
+        <v>18.8010093</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E19" s="8">
+        <f>MEDIAN(E8:E17)</f>
+        <v>1.3639035000000002</v>
+      </c>
+      <c r="F19" s="8">
+        <f>MEDIAN(F8:F17)</f>
+        <v>0.1029935</v>
+      </c>
+      <c r="G19" s="8">
+        <f>MEDIAN(G8:G17)</f>
+        <v>18.3993775</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>5315</v>
+      </c>
+      <c r="B21">
+        <v>5315</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1.358501</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.10315299999999999</v>
+      </c>
+      <c r="G21" s="2">
+        <v>17.074621</v>
+      </c>
+      <c r="H21" s="2">
+        <v>9.5316999999999999E-2</v>
+      </c>
+      <c r="I21" s="2">
+        <v>5.6634999999999998E-2</v>
+      </c>
       <c r="J21">
         <v>42</v>
       </c>
-    </row>
-    <row r="22" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="K21">
+        <v>100</v>
+      </c>
+      <c r="L21">
+        <v>50</v>
+      </c>
+      <c r="M21" t="s">
+        <v>33</v>
+      </c>
+      <c r="N21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E22" s="2">
+        <v>1.2587740000000001</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.101523</v>
+      </c>
+      <c r="G22" s="2">
+        <v>17.130113000000001</v>
+      </c>
+      <c r="H22" s="2">
+        <v>9.3073000000000003E-2</v>
+      </c>
+      <c r="I22" s="2">
+        <v>5.663E-2</v>
+      </c>
       <c r="J22">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="K22">
+        <v>100</v>
+      </c>
+      <c r="L22">
+        <v>50</v>
+      </c>
+      <c r="M22" t="s">
+        <v>33</v>
+      </c>
+      <c r="N22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E23" s="2">
+        <v>1.3292029999999999</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.108242</v>
+      </c>
+      <c r="G23" s="2">
+        <v>18.423794000000001</v>
+      </c>
+      <c r="H23" s="2">
+        <v>9.7717999999999999E-2</v>
+      </c>
+      <c r="I23" s="2">
+        <v>6.1550000000000001E-2</v>
+      </c>
       <c r="J23">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="K23">
+        <v>100</v>
+      </c>
+      <c r="L23">
+        <v>50</v>
+      </c>
+      <c r="M23" t="s">
+        <v>33</v>
+      </c>
+      <c r="N23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E24" s="2">
+        <v>1.300292</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.10151499999999999</v>
+      </c>
+      <c r="G24" s="2">
+        <v>17.941801000000002</v>
+      </c>
+      <c r="H24" s="2">
+        <v>9.3177999999999997E-2</v>
+      </c>
+      <c r="I24" s="2">
+        <v>5.7950000000000002E-2</v>
+      </c>
       <c r="J24">
         <v>45</v>
       </c>
-    </row>
-    <row r="25" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="K24">
+        <v>100</v>
+      </c>
+      <c r="L24">
+        <v>50</v>
+      </c>
+      <c r="M24" t="s">
+        <v>33</v>
+      </c>
+      <c r="N24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E25" s="2">
+        <v>1.375985</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.104336</v>
+      </c>
+      <c r="G25" s="2">
+        <v>17.559214000000001</v>
+      </c>
+      <c r="H25" s="2">
+        <v>9.5285999999999996E-2</v>
+      </c>
+      <c r="I25" s="2">
+        <v>5.6633000000000003E-2</v>
+      </c>
       <c r="J25">
         <v>46</v>
       </c>
-    </row>
-    <row r="26" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="K25">
+        <v>100</v>
+      </c>
+      <c r="L25">
+        <v>50</v>
+      </c>
+      <c r="M25" t="s">
+        <v>33</v>
+      </c>
+      <c r="N25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E26" s="2">
+        <v>1.768006</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.116618</v>
+      </c>
+      <c r="G26" s="2">
+        <v>21.680005000000001</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.110046</v>
+      </c>
+      <c r="I26" s="2">
+        <v>6.6986000000000004E-2</v>
+      </c>
       <c r="J26">
         <v>47</v>
       </c>
-    </row>
-    <row r="27" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="K26">
+        <v>100</v>
+      </c>
+      <c r="L26">
+        <v>50</v>
+      </c>
+      <c r="M26" t="s">
+        <v>33</v>
+      </c>
+      <c r="N26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E27" s="2">
+        <v>1.298041</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.102741</v>
+      </c>
+      <c r="G27" s="2">
+        <v>17.7545</v>
+      </c>
+      <c r="H27" s="2">
+        <v>9.3966999999999995E-2</v>
+      </c>
+      <c r="I27" s="2">
+        <v>5.5780999999999997E-2</v>
+      </c>
       <c r="J27">
         <v>48</v>
       </c>
-    </row>
-    <row r="28" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="K27">
+        <v>100</v>
+      </c>
+      <c r="L27">
+        <v>50</v>
+      </c>
+      <c r="M27" t="s">
+        <v>33</v>
+      </c>
+      <c r="N27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E28" s="2">
+        <v>1.3374159999999999</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0.104273</v>
+      </c>
+      <c r="G28" s="2">
+        <v>16.857208</v>
+      </c>
+      <c r="H28" s="2">
+        <v>9.4255000000000005E-2</v>
+      </c>
+      <c r="I28" s="2">
+        <v>5.7366E-2</v>
+      </c>
       <c r="J28">
         <v>49</v>
       </c>
+      <c r="K28">
+        <v>100</v>
+      </c>
+      <c r="L28">
+        <v>50</v>
+      </c>
+      <c r="M28" t="s">
+        <v>33</v>
+      </c>
+      <c r="N28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E29" s="2">
+        <v>1.5140199999999999</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.10766000000000001</v>
+      </c>
+      <c r="G29" s="2">
+        <v>18.054183999999999</v>
+      </c>
+      <c r="H29" s="2">
+        <v>9.7390000000000004E-2</v>
+      </c>
+      <c r="I29" s="2">
+        <v>5.7933999999999999E-2</v>
+      </c>
+      <c r="J29">
+        <v>50</v>
+      </c>
+      <c r="K29">
+        <v>100</v>
+      </c>
+      <c r="L29">
+        <v>50</v>
+      </c>
+      <c r="M29" t="s">
+        <v>33</v>
+      </c>
+      <c r="N29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E30" s="2">
+        <v>1.4592050000000001</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.106864</v>
+      </c>
+      <c r="G30" s="2">
+        <v>17.921873000000001</v>
+      </c>
+      <c r="H30" s="2">
+        <v>9.5794000000000004E-2</v>
+      </c>
+      <c r="I30" s="2">
+        <v>5.7357999999999999E-2</v>
+      </c>
+      <c r="J30">
+        <v>51</v>
+      </c>
+      <c r="K30">
+        <v>100</v>
+      </c>
+      <c r="L30">
+        <v>50</v>
+      </c>
+      <c r="M30" t="s">
+        <v>33</v>
+      </c>
+      <c r="N30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E31" s="8">
+        <f>AVERAGE(E21:E30)</f>
+        <v>1.3999443</v>
+      </c>
+      <c r="F31" s="8">
+        <f>AVERAGE(F21:F30)</f>
+        <v>0.10569249999999999</v>
+      </c>
+      <c r="G31" s="8">
+        <f>AVERAGE(G21:G30)</f>
+        <v>18.039731300000003</v>
+      </c>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E32" s="8">
+        <f>MEDIAN(E21:E30)</f>
+        <v>1.3479584999999998</v>
+      </c>
+      <c r="F32" s="8">
+        <f>MEDIAN(F21:F30)</f>
+        <v>0.10430449999999999</v>
+      </c>
+      <c r="G32" s="8">
+        <f>MEDIAN(G21:G30)</f>
+        <v>17.838186499999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>24000</v>
+      </c>
+      <c r="B34">
+        <v>5315</v>
+      </c>
+      <c r="C34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="2">
+        <v>1.2716099999999999</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0.10202</v>
+      </c>
+      <c r="G34" s="2">
+        <v>14.253511</v>
+      </c>
+      <c r="H34" s="2">
+        <v>9.1291999999999998E-2</v>
+      </c>
+      <c r="I34" s="2">
+        <v>5.2277999999999998E-2</v>
+      </c>
+      <c r="J34">
+        <v>42</v>
+      </c>
+      <c r="K34">
+        <v>200</v>
+      </c>
+      <c r="L34">
+        <v>100</v>
+      </c>
+      <c r="M34" t="s">
+        <v>32</v>
+      </c>
+      <c r="N34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E35" s="2">
+        <v>1.2456780000000001</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0.100775</v>
+      </c>
+      <c r="G35" s="2">
+        <v>16.773921999999999</v>
+      </c>
+      <c r="H35" s="2">
+        <v>9.2666999999999999E-2</v>
+      </c>
+      <c r="I35" s="2">
+        <v>5.4651999999999999E-2</v>
+      </c>
+      <c r="J35">
+        <v>43</v>
+      </c>
+      <c r="K35">
+        <v>200</v>
+      </c>
+      <c r="L35">
+        <v>100</v>
+      </c>
+      <c r="M35" t="s">
+        <v>32</v>
+      </c>
+      <c r="N35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E36" s="2">
+        <v>1.3031969999999999</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.104855</v>
+      </c>
+      <c r="G36" s="2">
+        <v>17.688960999999999</v>
+      </c>
+      <c r="H36" s="2">
+        <v>9.5528000000000002E-2</v>
+      </c>
+      <c r="I36" s="2">
+        <v>5.7931000000000003E-2</v>
+      </c>
+      <c r="J36">
+        <v>44</v>
+      </c>
+      <c r="K36">
+        <v>200</v>
+      </c>
+      <c r="L36">
+        <v>100</v>
+      </c>
+      <c r="M36" t="s">
+        <v>32</v>
+      </c>
+      <c r="N36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E37" s="2">
+        <v>1.2770649999999999</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.10112699999999999</v>
+      </c>
+      <c r="G37" s="2">
+        <v>18.051791000000001</v>
+      </c>
+      <c r="H37" s="2">
+        <v>9.2856999999999995E-2</v>
+      </c>
+      <c r="I37" s="2">
+        <v>5.7511E-2</v>
+      </c>
+      <c r="J37">
+        <v>45</v>
+      </c>
+      <c r="K37">
+        <v>200</v>
+      </c>
+      <c r="L37">
+        <v>100</v>
+      </c>
+      <c r="M37" t="s">
+        <v>32</v>
+      </c>
+      <c r="N37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E38" s="2">
+        <v>1.431792</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0.108058</v>
+      </c>
+      <c r="G38" s="2">
+        <v>16.557535000000001</v>
+      </c>
+      <c r="H38" s="2">
+        <v>9.8751000000000005E-2</v>
+      </c>
+      <c r="I38" s="2">
+        <v>5.7131000000000001E-2</v>
+      </c>
+      <c r="J38">
+        <v>46</v>
+      </c>
+      <c r="K38">
+        <v>200</v>
+      </c>
+      <c r="L38">
+        <v>100</v>
+      </c>
+      <c r="M38" t="s">
+        <v>32</v>
+      </c>
+      <c r="N38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E39" s="2">
+        <v>1.291933</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0.10190399999999999</v>
+      </c>
+      <c r="G39" s="2">
+        <v>18.873182</v>
+      </c>
+      <c r="H39" s="2">
+        <v>9.3701000000000007E-2</v>
+      </c>
+      <c r="I39" s="2">
+        <v>5.7062000000000002E-2</v>
+      </c>
+      <c r="J39">
+        <v>47</v>
+      </c>
+      <c r="K39">
+        <v>200</v>
+      </c>
+      <c r="L39">
+        <v>100</v>
+      </c>
+      <c r="M39" t="s">
+        <v>32</v>
+      </c>
+      <c r="N39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E40" s="2">
+        <v>1.3916790000000001</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0.10635</v>
+      </c>
+      <c r="G40" s="2">
+        <v>17.402757000000001</v>
+      </c>
+      <c r="H40" s="2">
+        <v>9.9541000000000004E-2</v>
+      </c>
+      <c r="I40" s="2">
+        <v>5.9199000000000002E-2</v>
+      </c>
+      <c r="J40">
+        <v>48</v>
+      </c>
+      <c r="K40">
+        <v>200</v>
+      </c>
+      <c r="L40">
+        <v>100</v>
+      </c>
+      <c r="M40" t="s">
+        <v>32</v>
+      </c>
+      <c r="N40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E41" s="2">
+        <v>1.3002659999999999</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0.10342700000000001</v>
+      </c>
+      <c r="G41" s="2">
+        <v>16.862074</v>
+      </c>
+      <c r="H41" s="2">
+        <v>9.4767000000000004E-2</v>
+      </c>
+      <c r="I41" s="2">
+        <v>5.5761999999999999E-2</v>
+      </c>
+      <c r="J41">
+        <v>49</v>
+      </c>
+      <c r="K41">
+        <v>200</v>
+      </c>
+      <c r="L41">
+        <v>100</v>
+      </c>
+      <c r="M41" t="s">
+        <v>32</v>
+      </c>
+      <c r="N41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E42" s="2">
+        <v>1.3325800000000001</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0.103065</v>
+      </c>
+      <c r="G42" s="2">
+        <v>18.362522999999999</v>
+      </c>
+      <c r="H42" s="2">
+        <v>9.4280000000000003E-2</v>
+      </c>
+      <c r="I42" s="2">
+        <v>5.5759999999999997E-2</v>
+      </c>
+      <c r="J42">
+        <v>50</v>
+      </c>
+      <c r="K42">
+        <v>200</v>
+      </c>
+      <c r="L42">
+        <v>100</v>
+      </c>
+      <c r="M42" t="s">
+        <v>32</v>
+      </c>
+      <c r="N42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E43" s="2">
+        <v>1.301293</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.10298499999999999</v>
+      </c>
+      <c r="G43" s="2">
+        <v>17.74408</v>
+      </c>
+      <c r="H43" s="2">
+        <v>9.4339999999999993E-2</v>
+      </c>
+      <c r="I43" s="2">
+        <v>5.7092999999999998E-2</v>
+      </c>
+      <c r="J43">
+        <v>51</v>
+      </c>
+      <c r="K43">
+        <v>200</v>
+      </c>
+      <c r="L43">
+        <v>100</v>
+      </c>
+      <c r="M43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E44" s="8">
+        <f>AVERAGE(E34:E43)</f>
+        <v>1.3147093000000001</v>
+      </c>
+      <c r="F44" s="8">
+        <f>AVERAGE(F34:F43)</f>
+        <v>0.10345659999999998</v>
+      </c>
+      <c r="G44" s="8">
+        <f>AVERAGE(G34:G43)</f>
+        <v>17.2570336</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E45" s="8">
+        <f>MEDIAN(E34:E43)</f>
+        <v>1.3007795</v>
+      </c>
+      <c r="F45" s="8">
+        <f>MEDIAN(F34:F43)</f>
+        <v>0.10302500000000001</v>
+      </c>
+      <c r="G45" s="8">
+        <f>MEDIAN(G34:G43)</f>
+        <v>17.545859</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>5315</v>
+      </c>
+      <c r="B47">
+        <v>5315</v>
+      </c>
+      <c r="C47" t="s">
+        <v>34</v>
+      </c>
+      <c r="E47" s="2">
+        <v>1.227166</v>
+      </c>
+      <c r="F47" s="2">
+        <v>9.9875000000000005E-2</v>
+      </c>
+      <c r="G47" s="2">
+        <v>10.926596</v>
+      </c>
+      <c r="H47" s="2">
+        <v>9.0494000000000005E-2</v>
+      </c>
+      <c r="I47" s="2">
+        <v>5.0380000000000001E-2</v>
+      </c>
+      <c r="J47">
+        <v>42</v>
+      </c>
+      <c r="K47">
+        <v>200</v>
+      </c>
+      <c r="L47">
+        <v>100</v>
+      </c>
+      <c r="M47" t="s">
+        <v>33</v>
+      </c>
+      <c r="N47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E48" s="2">
+        <v>1.2231719999999999</v>
+      </c>
+      <c r="F48" s="2">
+        <v>9.9956000000000003E-2</v>
+      </c>
+      <c r="G48" s="2">
+        <v>11.151490000000001</v>
+      </c>
+      <c r="H48" s="2">
+        <v>9.0811000000000003E-2</v>
+      </c>
+      <c r="I48" s="2">
+        <v>5.2971999999999998E-2</v>
+      </c>
+      <c r="J48">
+        <v>43</v>
+      </c>
+      <c r="K48">
+        <v>200</v>
+      </c>
+      <c r="L48">
+        <v>100</v>
+      </c>
+      <c r="M48" t="s">
+        <v>33</v>
+      </c>
+      <c r="N48" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E49" s="2">
+        <v>1.2898540000000001</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0.101005</v>
+      </c>
+      <c r="G49" s="2">
+        <v>11.661880999999999</v>
+      </c>
+      <c r="H49" s="2">
+        <v>9.2327999999999993E-2</v>
+      </c>
+      <c r="I49" s="2">
+        <v>5.1121E-2</v>
+      </c>
+      <c r="J49">
+        <v>44</v>
+      </c>
+      <c r="K49">
+        <v>200</v>
+      </c>
+      <c r="L49">
+        <v>100</v>
+      </c>
+      <c r="M49" t="s">
+        <v>33</v>
+      </c>
+      <c r="N49" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E50" s="2">
+        <v>1.21922</v>
+      </c>
+      <c r="F50" s="2">
+        <v>9.9584000000000006E-2</v>
+      </c>
+      <c r="G50" s="2">
+        <v>13.157942</v>
+      </c>
+      <c r="H50" s="2">
+        <v>9.0871999999999994E-2</v>
+      </c>
+      <c r="I50" s="2">
+        <v>5.0179000000000001E-2</v>
+      </c>
+      <c r="J50">
+        <v>45</v>
+      </c>
+      <c r="K50">
+        <v>200</v>
+      </c>
+      <c r="L50">
+        <v>100</v>
+      </c>
+      <c r="M50" t="s">
+        <v>33</v>
+      </c>
+      <c r="N50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E51" s="2">
+        <v>1.2339720000000001</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0.100038</v>
+      </c>
+      <c r="G51" s="2">
+        <v>12.262454</v>
+      </c>
+      <c r="H51" s="2">
+        <v>9.1045000000000001E-2</v>
+      </c>
+      <c r="I51" s="2">
+        <v>5.0056999999999997E-2</v>
+      </c>
+      <c r="J51">
+        <v>46</v>
+      </c>
+      <c r="K51">
+        <v>200</v>
+      </c>
+      <c r="L51">
+        <v>100</v>
+      </c>
+      <c r="M51" t="s">
+        <v>33</v>
+      </c>
+      <c r="N51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E52" s="2">
+        <v>1.2254119999999999</v>
+      </c>
+      <c r="F52" s="2">
+        <v>9.9856E-2</v>
+      </c>
+      <c r="G52" s="2">
+        <v>13.422684</v>
+      </c>
+      <c r="H52" s="2">
+        <v>9.0788999999999995E-2</v>
+      </c>
+      <c r="I52" s="2">
+        <v>5.1976000000000001E-2</v>
+      </c>
+      <c r="J52">
+        <v>47</v>
+      </c>
+      <c r="K52">
+        <v>200</v>
+      </c>
+      <c r="L52">
+        <v>100</v>
+      </c>
+      <c r="M52" t="s">
+        <v>33</v>
+      </c>
+      <c r="N52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E53" s="2">
+        <v>1.2274369999999999</v>
+      </c>
+      <c r="F53" s="2">
+        <v>9.9432000000000006E-2</v>
+      </c>
+      <c r="G53" s="2">
+        <v>11.58952</v>
+      </c>
+      <c r="H53" s="2">
+        <v>9.0316999999999995E-2</v>
+      </c>
+      <c r="I53" s="2">
+        <v>4.9641999999999999E-2</v>
+      </c>
+      <c r="J53">
+        <v>48</v>
+      </c>
+      <c r="K53">
+        <v>200</v>
+      </c>
+      <c r="L53">
+        <v>100</v>
+      </c>
+      <c r="M53" t="s">
+        <v>33</v>
+      </c>
+      <c r="N53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E54" s="2">
+        <v>1.490267</v>
+      </c>
+      <c r="F54" s="2">
+        <v>0.10815900000000001</v>
+      </c>
+      <c r="G54" s="2">
+        <v>17.387664000000001</v>
+      </c>
+      <c r="H54" s="2">
+        <v>9.9099000000000007E-2</v>
+      </c>
+      <c r="I54" s="2">
+        <v>5.7689999999999998E-2</v>
+      </c>
+      <c r="J54">
+        <v>49</v>
+      </c>
+      <c r="K54">
+        <v>200</v>
+      </c>
+      <c r="L54">
+        <v>100</v>
+      </c>
+      <c r="M54" t="s">
+        <v>33</v>
+      </c>
+      <c r="N54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E55" s="2">
+        <v>1.21071</v>
+      </c>
+      <c r="F55" s="2">
+        <v>9.8474999999999993E-2</v>
+      </c>
+      <c r="G55" s="2">
+        <v>11.018692</v>
+      </c>
+      <c r="H55" s="2">
+        <v>8.9592000000000005E-2</v>
+      </c>
+      <c r="I55" s="2">
+        <v>5.0358E-2</v>
+      </c>
+      <c r="J55">
+        <v>50</v>
+      </c>
+      <c r="K55">
+        <v>200</v>
+      </c>
+      <c r="L55">
+        <v>100</v>
+      </c>
+      <c r="M55" t="s">
+        <v>33</v>
+      </c>
+      <c r="N55" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E56" s="2">
+        <v>1.3010969999999999</v>
+      </c>
+      <c r="F56" s="2">
+        <v>0.103662</v>
+      </c>
+      <c r="G56" s="2">
+        <v>11.752516</v>
+      </c>
+      <c r="H56" s="2">
+        <v>9.5394999999999994E-2</v>
+      </c>
+      <c r="I56" s="2">
+        <v>5.3394999999999998E-2</v>
+      </c>
+      <c r="J56">
+        <v>51</v>
+      </c>
+      <c r="K56">
+        <v>200</v>
+      </c>
+      <c r="L56">
+        <v>100</v>
+      </c>
+      <c r="M56" t="s">
+        <v>33</v>
+      </c>
+      <c r="N56" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E57" s="8">
+        <f>AVERAGE(E47:E56)</f>
+        <v>1.2648307000000001</v>
+      </c>
+      <c r="F57" s="8">
+        <f>AVERAGE(F47:F56)</f>
+        <v>0.10100419999999999</v>
+      </c>
+      <c r="G57" s="8">
+        <f>AVERAGE(G47:G56)</f>
+        <v>12.433143899999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E58" s="8">
+        <f>MEDIAN(E47:E56)</f>
+        <v>1.2273014999999998</v>
+      </c>
+      <c r="F58" s="8">
+        <f>MEDIAN(F47:F56)</f>
+        <v>9.9915500000000004E-2</v>
+      </c>
+      <c r="G58" s="8">
+        <f>MEDIAN(G47:G56)</f>
+        <v>11.707198500000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>24000</v>
+      </c>
+      <c r="B60">
+        <v>5315</v>
+      </c>
+      <c r="C60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E60" s="2">
+        <v>1.2210399999999999</v>
+      </c>
+      <c r="F60" s="2">
+        <v>9.9048999999999998E-2</v>
+      </c>
+      <c r="G60" s="2">
+        <v>10.839835000000001</v>
+      </c>
+      <c r="H60" s="2">
+        <v>8.9190000000000005E-2</v>
+      </c>
+      <c r="I60" s="2">
+        <v>5.0402000000000002E-2</v>
+      </c>
+      <c r="J60">
+        <v>42</v>
+      </c>
+      <c r="K60">
+        <v>400</v>
+      </c>
+      <c r="L60">
+        <v>200</v>
+      </c>
+      <c r="M60" t="s">
+        <v>32</v>
+      </c>
+      <c r="N60" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E61" s="2">
+        <v>1.283174</v>
+      </c>
+      <c r="F61" s="2">
+        <v>0.100619</v>
+      </c>
+      <c r="G61" s="2">
+        <v>12.995926000000001</v>
+      </c>
+      <c r="H61" s="2">
+        <v>9.0794E-2</v>
+      </c>
+      <c r="I61" s="2">
+        <v>5.1499999999999997E-2</v>
+      </c>
+      <c r="J61">
+        <v>43</v>
+      </c>
+      <c r="K61">
+        <v>400</v>
+      </c>
+      <c r="L61">
+        <v>200</v>
+      </c>
+      <c r="M61" t="s">
+        <v>32</v>
+      </c>
+      <c r="N61" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E62" s="2">
+        <v>1.2268079999999999</v>
+      </c>
+      <c r="F62" s="2">
+        <v>9.8169000000000006E-2</v>
+      </c>
+      <c r="G62" s="2">
+        <v>12.394558999999999</v>
+      </c>
+      <c r="H62" s="2">
+        <v>8.9478000000000002E-2</v>
+      </c>
+      <c r="I62" s="2">
+        <v>4.7779000000000002E-2</v>
+      </c>
+      <c r="J62">
+        <v>44</v>
+      </c>
+      <c r="K62">
+        <v>400</v>
+      </c>
+      <c r="L62">
+        <v>200</v>
+      </c>
+      <c r="M62" t="s">
+        <v>32</v>
+      </c>
+      <c r="N62" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E63" s="2">
+        <v>1.3577170000000001</v>
+      </c>
+      <c r="F63" s="2">
+        <v>0.10355</v>
+      </c>
+      <c r="G63" s="2">
+        <v>12.386239</v>
+      </c>
+      <c r="H63" s="2">
+        <v>9.4778000000000001E-2</v>
+      </c>
+      <c r="I63" s="2">
+        <v>5.1721999999999997E-2</v>
+      </c>
+      <c r="J63">
+        <v>45</v>
+      </c>
+      <c r="K63">
+        <v>400</v>
+      </c>
+      <c r="L63">
+        <v>200</v>
+      </c>
+      <c r="M63" t="s">
+        <v>32</v>
+      </c>
+      <c r="N63" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E64" s="2">
+        <v>1.2006220000000001</v>
+      </c>
+      <c r="F64" s="2">
+        <v>9.7045000000000006E-2</v>
+      </c>
+      <c r="G64" s="2">
+        <v>11.868323</v>
+      </c>
+      <c r="H64" s="2">
+        <v>8.7941000000000005E-2</v>
+      </c>
+      <c r="I64" s="2">
+        <v>4.6954000000000003E-2</v>
+      </c>
+      <c r="J64">
+        <v>46</v>
+      </c>
+      <c r="K64">
+        <v>400</v>
+      </c>
+      <c r="L64">
+        <v>200</v>
+      </c>
+      <c r="M64" t="s">
+        <v>32</v>
+      </c>
+      <c r="N64" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J67">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J68">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J69">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E70" s="8">
+        <f>AVERAGE(E60:E69)</f>
+        <v>1.2578722</v>
+      </c>
+      <c r="F70" s="8">
+        <f>AVERAGE(F60:F69)</f>
+        <v>9.9686400000000008E-2</v>
+      </c>
+      <c r="G70" s="8">
+        <f>AVERAGE(G60:G69)</f>
+        <v>12.096976399999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E71" s="8">
+        <f>MEDIAN(E60:E69)</f>
+        <v>1.2268079999999999</v>
+      </c>
+      <c r="F71" s="8">
+        <f>MEDIAN(F60:F69)</f>
+        <v>9.9048999999999998E-2</v>
+      </c>
+      <c r="G71" s="8">
+        <f>MEDIAN(G60:G69)</f>
+        <v>12.386239</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>5315</v>
+      </c>
+      <c r="B73">
+        <v>5315</v>
+      </c>
+      <c r="C73" t="s">
+        <v>34</v>
+      </c>
+      <c r="E73" s="2">
+        <v>1.2015849999999999</v>
+      </c>
+      <c r="F73" s="2">
+        <v>9.7647999999999999E-2</v>
+      </c>
+      <c r="G73" s="2">
+        <v>11.267737</v>
+      </c>
+      <c r="H73" s="2">
+        <v>8.8314000000000004E-2</v>
+      </c>
+      <c r="I73" s="2">
+        <v>4.7204000000000003E-2</v>
+      </c>
+      <c r="J73">
+        <v>42</v>
+      </c>
+      <c r="K73">
+        <v>400</v>
+      </c>
+      <c r="L73">
+        <v>200</v>
+      </c>
+      <c r="M73" t="s">
+        <v>33</v>
+      </c>
+      <c r="N73" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E74" s="2">
+        <v>1.195549</v>
+      </c>
+      <c r="F74" s="2">
+        <v>9.6995999999999999E-2</v>
+      </c>
+      <c r="G74" s="2">
+        <v>11.709352000000001</v>
+      </c>
+      <c r="H74" s="2">
+        <v>8.7660000000000002E-2</v>
+      </c>
+      <c r="I74" s="2">
+        <v>4.6574999999999998E-2</v>
+      </c>
+      <c r="J74">
+        <v>43</v>
+      </c>
+      <c r="K74">
+        <v>400</v>
+      </c>
+      <c r="L74">
+        <v>200</v>
+      </c>
+      <c r="M74" t="s">
+        <v>33</v>
+      </c>
+      <c r="N74" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E75" s="2">
+        <v>1.2322299999999999</v>
+      </c>
+      <c r="F75" s="2">
+        <v>9.8443000000000003E-2</v>
+      </c>
+      <c r="G75" s="2">
+        <v>11.739494000000001</v>
+      </c>
+      <c r="H75" s="2">
+        <v>8.8628999999999999E-2</v>
+      </c>
+      <c r="I75" s="2">
+        <v>4.7301999999999997E-2</v>
+      </c>
+      <c r="J75">
+        <v>44</v>
+      </c>
+      <c r="K75">
+        <v>400</v>
+      </c>
+      <c r="L75">
+        <v>200</v>
+      </c>
+      <c r="M75" t="s">
+        <v>33</v>
+      </c>
+      <c r="N75" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E76" s="2">
+        <v>1.1963729999999999</v>
+      </c>
+      <c r="F76" s="2">
+        <v>9.7239000000000006E-2</v>
+      </c>
+      <c r="G76" s="2">
+        <v>11.581034000000001</v>
+      </c>
+      <c r="H76" s="2">
+        <v>8.7625999999999996E-2</v>
+      </c>
+      <c r="I76" s="2">
+        <v>4.5738000000000001E-2</v>
+      </c>
+      <c r="J76">
+        <v>45</v>
+      </c>
+      <c r="K76">
+        <v>400</v>
+      </c>
+      <c r="L76">
+        <v>200</v>
+      </c>
+      <c r="M76" t="s">
+        <v>33</v>
+      </c>
+      <c r="N76" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E77" s="2">
+        <v>1.2327589999999999</v>
+      </c>
+      <c r="F77" s="2">
+        <v>9.8130999999999996E-2</v>
+      </c>
+      <c r="G77" s="2">
+        <v>11.942957</v>
+      </c>
+      <c r="H77" s="2">
+        <v>8.8562000000000002E-2</v>
+      </c>
+      <c r="I77" s="2">
+        <v>4.6276999999999999E-2</v>
+      </c>
+      <c r="J77">
+        <v>46</v>
+      </c>
+      <c r="K77">
+        <v>400</v>
+      </c>
+      <c r="L77">
+        <v>200</v>
+      </c>
+      <c r="M77" t="s">
+        <v>33</v>
+      </c>
+      <c r="N77" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J78">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J79">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J80">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J81">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J82">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E83" s="8">
+        <f>AVERAGE(E73:E82)</f>
+        <v>1.2116992</v>
+      </c>
+      <c r="F83" s="8">
+        <f>AVERAGE(F73:F82)</f>
+        <v>9.7691400000000012E-2</v>
+      </c>
+      <c r="G83" s="8">
+        <f>AVERAGE(G73:G82)</f>
+        <v>11.6481148</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E84" s="8">
+        <f>MEDIAN(E73:E82)</f>
+        <v>1.2015849999999999</v>
+      </c>
+      <c r="F84" s="8">
+        <f>MEDIAN(F73:F82)</f>
+        <v>9.7647999999999999E-2</v>
+      </c>
+      <c r="G84" s="8">
+        <f>MEDIAN(G73:G82)</f>
+        <v>11.709352000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>24000</v>
+      </c>
+      <c r="B86">
+        <v>5315</v>
+      </c>
+      <c r="C86" t="s">
+        <v>34</v>
+      </c>
+      <c r="E86" s="2">
+        <v>1.1941839999999999</v>
+      </c>
+      <c r="F86" s="2">
+        <v>9.8169999999999993E-2</v>
+      </c>
+      <c r="G86" s="2">
+        <v>11.312642</v>
+      </c>
+      <c r="H86" s="2">
+        <v>8.8293999999999997E-2</v>
+      </c>
+      <c r="I86" s="2">
+        <v>4.9801999999999999E-2</v>
+      </c>
+      <c r="J86">
+        <v>42</v>
+      </c>
+      <c r="K86">
+        <v>750</v>
+      </c>
+      <c r="L86">
+        <v>100</v>
+      </c>
+      <c r="M86" t="s">
+        <v>32</v>
+      </c>
+      <c r="N86" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E87" s="2">
+        <v>1.2419420000000001</v>
+      </c>
+      <c r="F87" s="2">
+        <v>9.9301E-2</v>
+      </c>
+      <c r="G87" s="2">
+        <v>12.376564</v>
+      </c>
+      <c r="H87" s="2">
+        <v>8.9590000000000003E-2</v>
+      </c>
+      <c r="I87" s="2">
+        <v>5.1059E-2</v>
+      </c>
+      <c r="J87">
+        <v>43</v>
+      </c>
+      <c r="K87">
+        <v>750</v>
+      </c>
+      <c r="L87">
+        <v>100</v>
+      </c>
+      <c r="M87" t="s">
+        <v>32</v>
+      </c>
+      <c r="N87" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E88" s="2">
+        <v>1.344635</v>
+      </c>
+      <c r="F88" s="2">
+        <v>0.10291699999999999</v>
+      </c>
+      <c r="G88" s="2">
+        <v>11.884278999999999</v>
+      </c>
+      <c r="H88" s="2">
+        <v>9.3661999999999995E-2</v>
+      </c>
+      <c r="I88" s="2">
+        <v>5.2219000000000002E-2</v>
+      </c>
+      <c r="J88">
+        <v>44</v>
+      </c>
+      <c r="K88">
+        <v>750</v>
+      </c>
+      <c r="L88">
+        <v>100</v>
+      </c>
+      <c r="M88" t="s">
+        <v>32</v>
+      </c>
+      <c r="N88" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J89">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J90">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J91">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J92">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J93">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J94">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J95">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E96" s="8">
+        <f>AVERAGE(E86:E95)</f>
+        <v>1.2602536666666666</v>
+      </c>
+      <c r="F96" s="8">
+        <f>AVERAGE(F86:F95)</f>
+        <v>0.10012933333333333</v>
+      </c>
+      <c r="G96" s="8">
+        <f>AVERAGE(G86:G95)</f>
+        <v>11.857828333333332</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E97" s="8">
+        <f>MEDIAN(E86:E95)</f>
+        <v>1.2419420000000001</v>
+      </c>
+      <c r="F97" s="8">
+        <f>MEDIAN(F86:F95)</f>
+        <v>9.9301E-2</v>
+      </c>
+      <c r="G97" s="8">
+        <f>MEDIAN(G86:G95)</f>
+        <v>11.884278999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>5315</v>
+      </c>
+      <c r="B99">
+        <v>5315</v>
+      </c>
+      <c r="C99" t="s">
+        <v>34</v>
+      </c>
+      <c r="E99" s="2">
+        <v>1.2289380000000001</v>
+      </c>
+      <c r="F99" s="2">
+        <v>9.9902000000000005E-2</v>
+      </c>
+      <c r="G99" s="2">
+        <v>10.933592000000001</v>
+      </c>
+      <c r="H99" s="2">
+        <v>9.0568999999999997E-2</v>
+      </c>
+      <c r="I99" s="2">
+        <v>5.0650000000000001E-2</v>
+      </c>
+      <c r="J99">
+        <v>42</v>
+      </c>
+      <c r="K99">
+        <v>167</v>
+      </c>
+      <c r="L99">
+        <v>100</v>
+      </c>
+      <c r="M99" t="s">
+        <v>33</v>
+      </c>
+      <c r="N99" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E100" s="2">
+        <v>1.2155469999999999</v>
+      </c>
+      <c r="F100" s="2">
+        <v>9.9349999999999994E-2</v>
+      </c>
+      <c r="G100" s="2">
+        <v>11.320676000000001</v>
+      </c>
+      <c r="H100" s="2">
+        <v>9.0053999999999995E-2</v>
+      </c>
+      <c r="I100" s="2">
+        <v>5.1943999999999997E-2</v>
+      </c>
+      <c r="J100">
+        <v>43</v>
+      </c>
+      <c r="K100">
+        <v>167</v>
+      </c>
+      <c r="L100">
+        <v>100</v>
+      </c>
+      <c r="M100" t="s">
+        <v>33</v>
+      </c>
+      <c r="N100" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E101" s="2">
+        <v>1.287112</v>
+      </c>
+      <c r="F101" s="2">
+        <v>0.100868</v>
+      </c>
+      <c r="G101" s="2">
+        <v>11.673899</v>
+      </c>
+      <c r="H101" s="2">
+        <v>9.2136999999999997E-2</v>
+      </c>
+      <c r="I101" s="2">
+        <v>5.1024E-2</v>
+      </c>
+      <c r="J101">
+        <v>44</v>
+      </c>
+      <c r="K101">
+        <v>167</v>
+      </c>
+      <c r="L101">
+        <v>100</v>
+      </c>
+      <c r="M101" t="s">
+        <v>33</v>
+      </c>
+      <c r="N101" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J102">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J103">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J104">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J105">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J106">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J107">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J108">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E109" s="8">
+        <f>AVERAGE(E99:E108)</f>
+        <v>1.2438656666666668</v>
+      </c>
+      <c r="F109" s="8">
+        <f>AVERAGE(F99:F108)</f>
+        <v>0.10004</v>
+      </c>
+      <c r="G109" s="8">
+        <f>AVERAGE(G99:G108)</f>
+        <v>11.309389000000001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E110" s="8">
+        <f>MEDIAN(E99:E108)</f>
+        <v>1.2289380000000001</v>
+      </c>
+      <c r="F110" s="8">
+        <f>MEDIAN(F99:F108)</f>
+        <v>9.9902000000000005E-2</v>
+      </c>
+      <c r="G110" s="8">
+        <f>MEDIAN(G99:G108)</f>
+        <v>11.320676000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{176A91C0-2D0B-461D-A2E7-3C52989DDACB}">
+  <dimension ref="A1:P70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E70" sqref="E70"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" customWidth="1"/>
+    <col min="5" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.54296875" customWidth="1"/>
+    <col min="13" max="13" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>24000</v>
+      </c>
+      <c r="B9">
+        <v>6020</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.304136</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.10857799999999999</v>
+      </c>
+      <c r="G9" s="2">
+        <v>19.277940999999998</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.10553999999999999</v>
+      </c>
+      <c r="I9" s="2">
+        <v>7.1210999999999997E-2</v>
+      </c>
+      <c r="J9">
+        <v>42</v>
+      </c>
+      <c r="K9">
+        <v>100</v>
+      </c>
+      <c r="L9">
+        <v>50</v>
+      </c>
+      <c r="M9" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E10" s="2">
+        <v>1.296916</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.10760400000000001</v>
+      </c>
+      <c r="G10" s="2">
+        <v>17.393923000000001</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.101284</v>
+      </c>
+      <c r="I10" s="2">
+        <v>6.6772999999999999E-2</v>
+      </c>
+      <c r="J10">
+        <v>43</v>
+      </c>
+      <c r="K10">
+        <v>100</v>
+      </c>
+      <c r="L10">
+        <v>50</v>
+      </c>
+      <c r="M10" t="s">
+        <v>32</v>
+      </c>
+      <c r="N10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E11" s="2">
+        <v>1.3391189999999999</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.109788</v>
+      </c>
+      <c r="G11" s="2">
+        <v>17.652006</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.105709</v>
+      </c>
+      <c r="I11" s="2">
+        <v>6.7237000000000005E-2</v>
+      </c>
+      <c r="J11">
+        <v>44</v>
+      </c>
+      <c r="K11">
+        <v>100</v>
+      </c>
+      <c r="L11">
+        <v>50</v>
+      </c>
+      <c r="M11" t="s">
+        <v>32</v>
+      </c>
+      <c r="N11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E12" s="2">
+        <v>1.355588</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.110273</v>
+      </c>
+      <c r="G12" s="2">
+        <v>21.458608000000002</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.108496</v>
+      </c>
+      <c r="I12" s="2">
+        <v>7.8941999999999998E-2</v>
+      </c>
+      <c r="J12">
+        <v>45</v>
+      </c>
+      <c r="K12">
+        <v>100</v>
+      </c>
+      <c r="L12">
+        <v>50</v>
+      </c>
+      <c r="M12" t="s">
+        <v>32</v>
+      </c>
+      <c r="N12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E13" s="2">
+        <v>1.3181659999999999</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.108621</v>
+      </c>
+      <c r="G13" s="2">
+        <v>17.807941</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.104409</v>
+      </c>
+      <c r="I13" s="2">
+        <v>6.9958000000000006E-2</v>
+      </c>
+      <c r="J13">
+        <v>46</v>
+      </c>
+      <c r="K13">
+        <v>100</v>
+      </c>
+      <c r="L13">
+        <v>50</v>
+      </c>
+      <c r="M13" t="s">
+        <v>32</v>
+      </c>
+      <c r="N13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E14" s="2">
+        <v>1.2964910000000001</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.108321</v>
+      </c>
+      <c r="G14" s="2">
+        <v>17.948761000000001</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.10642699999999999</v>
+      </c>
+      <c r="I14" s="2">
+        <v>7.0583000000000007E-2</v>
+      </c>
+      <c r="J14">
+        <v>47</v>
+      </c>
+      <c r="K14">
+        <v>100</v>
+      </c>
+      <c r="L14">
+        <v>50</v>
+      </c>
+      <c r="M14" t="s">
+        <v>32</v>
+      </c>
+      <c r="N14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E15" s="2">
+        <v>1.666725</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.121128</v>
+      </c>
+      <c r="G15" s="2">
+        <v>19.073461999999999</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.109468</v>
+      </c>
+      <c r="I15" s="2">
+        <v>6.5605999999999998E-2</v>
+      </c>
+      <c r="J15">
+        <v>48</v>
+      </c>
+      <c r="K15">
+        <v>100</v>
+      </c>
+      <c r="L15">
+        <v>50</v>
+      </c>
+      <c r="M15" t="s">
+        <v>32</v>
+      </c>
+      <c r="N15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E16" s="2">
+        <v>1.2863800000000001</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.10774</v>
+      </c>
+      <c r="G16" s="2">
+        <v>17.482453</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.103843</v>
+      </c>
+      <c r="I16" s="2">
+        <v>7.0736999999999994E-2</v>
+      </c>
+      <c r="J16">
+        <v>49</v>
+      </c>
+      <c r="K16">
+        <v>100</v>
+      </c>
+      <c r="L16">
+        <v>50</v>
+      </c>
+      <c r="M16" t="s">
+        <v>32</v>
+      </c>
+      <c r="N16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E17" s="2">
+        <v>1.3272660000000001</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.10910300000000001</v>
+      </c>
+      <c r="G17" s="2">
+        <v>19.842174</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.107211</v>
+      </c>
+      <c r="I17" s="2">
+        <v>7.5228000000000003E-2</v>
+      </c>
+      <c r="J17">
+        <v>50</v>
+      </c>
+      <c r="K17">
+        <v>100</v>
+      </c>
+      <c r="L17">
+        <v>50</v>
+      </c>
+      <c r="M17" t="s">
+        <v>32</v>
+      </c>
+      <c r="N17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E18" s="2">
+        <v>1.3503890000000001</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.110017</v>
+      </c>
+      <c r="G18" s="2">
+        <v>17.855301000000001</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.10861</v>
+      </c>
+      <c r="I18" s="2">
+        <v>7.0001999999999995E-2</v>
+      </c>
+      <c r="J18">
+        <v>51</v>
+      </c>
+      <c r="K18">
+        <v>100</v>
+      </c>
+      <c r="L18">
+        <v>50</v>
+      </c>
+      <c r="M18" t="s">
+        <v>32</v>
+      </c>
+      <c r="N18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E22" s="2">
+        <v>1.4056390000000001</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.11117299999999999</v>
+      </c>
+      <c r="G22" s="2">
+        <v>18.980537999999999</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0.10360999999999999</v>
+      </c>
+      <c r="I22" s="2">
+        <v>6.5434999999999993E-2</v>
+      </c>
+      <c r="J22">
+        <v>42</v>
+      </c>
+      <c r="K22">
+        <v>100</v>
+      </c>
+      <c r="L22">
+        <v>50</v>
+      </c>
+      <c r="M22" t="s">
+        <v>37</v>
+      </c>
+      <c r="N22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E23" s="2">
+        <v>1.3042309999999999</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.108114</v>
+      </c>
+      <c r="G23" s="2">
+        <v>17.795528999999998</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.102494</v>
+      </c>
+      <c r="I23" s="2">
+        <v>6.7483000000000001E-2</v>
+      </c>
+      <c r="J23">
+        <v>43</v>
+      </c>
+      <c r="K23">
+        <v>100</v>
+      </c>
+      <c r="L23">
+        <v>50</v>
+      </c>
+      <c r="M23" t="s">
+        <v>37</v>
+      </c>
+      <c r="N23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E24" s="2">
+        <v>1.260734</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.106404</v>
+      </c>
+      <c r="G24" s="2">
+        <v>16.191579999999998</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.10134</v>
+      </c>
+      <c r="I24" s="2">
+        <v>6.5232999999999999E-2</v>
+      </c>
+      <c r="J24">
+        <v>44</v>
+      </c>
+      <c r="K24">
+        <v>100</v>
+      </c>
+      <c r="L24">
+        <v>50</v>
+      </c>
+      <c r="M24" t="s">
+        <v>37</v>
+      </c>
+      <c r="N24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E25" s="2">
+        <v>1.4030119999999999</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.111882</v>
+      </c>
+      <c r="G25" s="2">
+        <v>17.796036000000001</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.110939</v>
+      </c>
+      <c r="I25" s="2">
+        <v>7.0667999999999995E-2</v>
+      </c>
+      <c r="J25">
+        <v>45</v>
+      </c>
+      <c r="K25">
+        <v>100</v>
+      </c>
+      <c r="L25">
+        <v>50</v>
+      </c>
+      <c r="M25" t="s">
+        <v>37</v>
+      </c>
+      <c r="N25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E26" s="2">
+        <v>1.255698</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.10725</v>
+      </c>
+      <c r="G26" s="2">
+        <v>16.76567</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.10309599999999999</v>
+      </c>
+      <c r="I26" s="2">
+        <v>6.3562999999999995E-2</v>
+      </c>
+      <c r="J26">
+        <v>46</v>
+      </c>
+      <c r="K26">
+        <v>100</v>
+      </c>
+      <c r="L26">
+        <v>50</v>
+      </c>
+      <c r="M26" t="s">
+        <v>37</v>
+      </c>
+      <c r="N26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E27" s="2">
+        <v>2.105855</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.13677600000000001</v>
+      </c>
+      <c r="G27" s="2">
+        <v>28.665775</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0.126557</v>
+      </c>
+      <c r="I27" s="2">
+        <v>6.6326999999999997E-2</v>
+      </c>
+      <c r="J27">
+        <v>47</v>
+      </c>
+      <c r="K27">
+        <v>100</v>
+      </c>
+      <c r="L27">
+        <v>50</v>
+      </c>
+      <c r="M27" t="s">
+        <v>37</v>
+      </c>
+      <c r="N27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E28" s="2">
+        <v>1.2659929999999999</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0.106514</v>
+      </c>
+      <c r="G28" s="2">
+        <v>17.418588</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0.10274899999999999</v>
+      </c>
+      <c r="I28" s="2">
+        <v>6.6770999999999997E-2</v>
+      </c>
+      <c r="J28">
+        <v>48</v>
+      </c>
+      <c r="K28">
+        <v>100</v>
+      </c>
+      <c r="L28">
+        <v>50</v>
+      </c>
+      <c r="M28" t="s">
+        <v>37</v>
+      </c>
+      <c r="N28" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="29" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E29" s="2">
+        <v>1.330225</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.108557</v>
+      </c>
+      <c r="G29" s="2">
+        <v>18.019432999999999</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0.102644</v>
+      </c>
+      <c r="I29" s="2">
+        <v>6.8840999999999999E-2</v>
+      </c>
       <c r="J29">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="K29">
+        <v>100</v>
+      </c>
+      <c r="L29">
+        <v>50</v>
+      </c>
+      <c r="M29" t="s">
+        <v>37</v>
+      </c>
+      <c r="N29" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E30" s="2">
+        <v>1.288904</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.106889</v>
+      </c>
+      <c r="G30" s="2">
+        <v>16.220293999999999</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0.10316699999999999</v>
+      </c>
+      <c r="I30" s="2">
+        <v>6.5299999999999997E-2</v>
+      </c>
       <c r="J30">
+        <v>50</v>
+      </c>
+      <c r="K30">
+        <v>100</v>
+      </c>
+      <c r="L30">
+        <v>50</v>
+      </c>
+      <c r="M30" t="s">
+        <v>37</v>
+      </c>
+      <c r="N30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E31" s="2">
+        <v>1.359418</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.109343</v>
+      </c>
+      <c r="G31" s="2">
+        <v>16.591812999999998</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0.103545</v>
+      </c>
+      <c r="I31" s="2">
+        <v>6.6388000000000003E-2</v>
+      </c>
+      <c r="J31">
+        <v>51</v>
+      </c>
+      <c r="K31">
+        <v>100</v>
+      </c>
+      <c r="L31">
+        <v>50</v>
+      </c>
+      <c r="M31" t="s">
+        <v>37</v>
+      </c>
+      <c r="N31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>24000</v>
+      </c>
+      <c r="B35">
+        <v>6020</v>
+      </c>
+      <c r="C35" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="2">
+        <v>1.2584390000000001</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0.10861</v>
+      </c>
+      <c r="G35" s="2">
+        <v>14.736345999999999</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0.102468</v>
+      </c>
+      <c r="I35" s="2">
+        <v>6.055E-2</v>
+      </c>
+      <c r="J35">
+        <v>42</v>
+      </c>
+      <c r="K35">
+        <v>200</v>
+      </c>
+      <c r="L35">
+        <v>100</v>
+      </c>
+      <c r="M35" t="s">
+        <v>32</v>
+      </c>
+      <c r="N35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E36" s="2">
+        <v>1.2131730000000001</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.105392</v>
+      </c>
+      <c r="G36" s="2">
+        <v>16.244857</v>
+      </c>
+      <c r="H36" s="2">
+        <v>9.9455000000000002E-2</v>
+      </c>
+      <c r="I36" s="2">
+        <v>6.3242999999999994E-2</v>
+      </c>
+      <c r="J36">
+        <v>43</v>
+      </c>
+      <c r="K36">
+        <v>200</v>
+      </c>
+      <c r="L36">
+        <v>100</v>
+      </c>
+      <c r="M36" t="s">
+        <v>32</v>
+      </c>
+      <c r="N36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E37" s="2">
+        <v>1.2447779999999999</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.10732</v>
+      </c>
+      <c r="G37" s="2">
+        <v>16.640418</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0.100951</v>
+      </c>
+      <c r="I37" s="2">
+        <v>6.5882999999999997E-2</v>
+      </c>
+      <c r="J37">
+        <v>44</v>
+      </c>
+      <c r="K37">
+        <v>200</v>
+      </c>
+      <c r="L37">
+        <v>100</v>
+      </c>
+      <c r="M37" t="s">
+        <v>32</v>
+      </c>
+      <c r="N37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E38" s="2">
+        <v>1.2869969999999999</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0.108096</v>
+      </c>
+      <c r="G38" s="2">
+        <v>18.441678</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0.105504</v>
+      </c>
+      <c r="I38" s="2">
+        <v>7.0900000000000005E-2</v>
+      </c>
+      <c r="J38">
+        <v>45</v>
+      </c>
+      <c r="K38">
+        <v>200</v>
+      </c>
+      <c r="L38">
+        <v>100</v>
+      </c>
+      <c r="M38" t="s">
+        <v>32</v>
+      </c>
+      <c r="N38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E39" s="2">
+        <v>1.3393520000000001</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0.11156099999999999</v>
+      </c>
+      <c r="G39" s="2">
+        <v>16.188078000000001</v>
+      </c>
+      <c r="H39" s="2">
+        <v>0.103784</v>
+      </c>
+      <c r="I39" s="2">
+        <v>6.4739000000000005E-2</v>
+      </c>
+      <c r="J39">
+        <v>46</v>
+      </c>
+      <c r="K39">
+        <v>200</v>
+      </c>
+      <c r="L39">
+        <v>100</v>
+      </c>
+      <c r="M39" t="s">
+        <v>32</v>
+      </c>
+      <c r="N39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E40" s="2">
+        <v>1.2708170000000001</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0.107241</v>
+      </c>
+      <c r="G40" s="2">
+        <v>18.831598</v>
+      </c>
+      <c r="H40" s="2">
+        <v>0.10347000000000001</v>
+      </c>
+      <c r="I40" s="2">
+        <v>7.0306999999999994E-2</v>
+      </c>
+      <c r="J40">
+        <v>47</v>
+      </c>
+      <c r="K40">
+        <v>200</v>
+      </c>
+      <c r="L40">
+        <v>100</v>
+      </c>
+      <c r="M40" t="s">
+        <v>32</v>
+      </c>
+      <c r="N40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E41" s="2">
+        <v>1.274519</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0.107532</v>
+      </c>
+      <c r="G41" s="2">
+        <v>16.100676</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0.10208</v>
+      </c>
+      <c r="I41" s="2">
+        <v>6.4648999999999998E-2</v>
+      </c>
+      <c r="J41">
+        <v>48</v>
+      </c>
+      <c r="K41">
+        <v>200</v>
+      </c>
+      <c r="L41">
+        <v>100</v>
+      </c>
+      <c r="M41" t="s">
+        <v>32</v>
+      </c>
+      <c r="N41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E42" s="2">
+        <v>1.2331179999999999</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0.106738</v>
+      </c>
+      <c r="G42" s="2">
+        <v>16.227595999999998</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0.10125099999999999</v>
+      </c>
+      <c r="I42" s="2">
+        <v>6.4613000000000004E-2</v>
+      </c>
+      <c r="J42">
+        <v>49</v>
+      </c>
+      <c r="K42">
+        <v>200</v>
+      </c>
+      <c r="L42">
+        <v>100</v>
+      </c>
+      <c r="M42" t="s">
+        <v>32</v>
+      </c>
+      <c r="N42" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E43" s="2">
+        <v>1.273879</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.10652</v>
+      </c>
+      <c r="G43" s="2">
+        <v>17.608233999999999</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0.101969</v>
+      </c>
+      <c r="I43" s="2">
+        <v>6.7029000000000005E-2</v>
+      </c>
+      <c r="J43">
+        <v>50</v>
+      </c>
+      <c r="K43">
+        <v>200</v>
+      </c>
+      <c r="L43">
+        <v>100</v>
+      </c>
+      <c r="M43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N43" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E44" s="2">
+        <v>1.229117</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0.105239</v>
+      </c>
+      <c r="G44" s="2">
+        <v>16.916333000000002</v>
+      </c>
+      <c r="H44" s="2">
+        <v>9.9192000000000002E-2</v>
+      </c>
+      <c r="I44" s="2">
+        <v>6.4702999999999997E-2</v>
+      </c>
+      <c r="J44">
+        <v>51</v>
+      </c>
+      <c r="K44">
+        <v>200</v>
+      </c>
+      <c r="L44">
+        <v>100</v>
+      </c>
+      <c r="M44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N44" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E48" s="2">
+        <v>1.232907</v>
+      </c>
+      <c r="F48" s="2">
+        <v>0.107297</v>
+      </c>
+      <c r="G48" s="2">
+        <v>13.561297</v>
+      </c>
+      <c r="H48" s="2">
+        <v>0.102321</v>
+      </c>
+      <c r="I48" s="2">
+        <v>5.7196999999999998E-2</v>
+      </c>
+      <c r="J48">
+        <v>42</v>
+      </c>
+      <c r="K48">
+        <v>200</v>
+      </c>
+      <c r="L48">
+        <v>100</v>
+      </c>
+      <c r="M48" t="s">
+        <v>37</v>
+      </c>
+      <c r="N48" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E49" s="2">
+        <v>1.436477</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0.113153</v>
+      </c>
+      <c r="G49" s="2">
+        <v>13.275743</v>
+      </c>
+      <c r="H49" s="2">
+        <v>0.10353900000000001</v>
+      </c>
+      <c r="I49" s="2">
+        <v>6.7229999999999998E-2</v>
+      </c>
+      <c r="J49">
+        <v>43</v>
+      </c>
+      <c r="K49">
+        <v>200</v>
+      </c>
+      <c r="L49">
+        <v>100</v>
+      </c>
+      <c r="M49" t="s">
+        <v>37</v>
+      </c>
+      <c r="N49" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E50" s="2">
+        <v>1.2421180000000001</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0.10559499999999999</v>
+      </c>
+      <c r="G50" s="2">
+        <v>16.307234000000001</v>
+      </c>
+      <c r="H50" s="2">
+        <v>0.100332</v>
+      </c>
+      <c r="I50" s="2">
+        <v>6.3772999999999996E-2</v>
+      </c>
+      <c r="J50">
+        <v>44</v>
+      </c>
+      <c r="K50">
+        <v>200</v>
+      </c>
+      <c r="L50">
+        <v>100</v>
+      </c>
+      <c r="M50" t="s">
+        <v>37</v>
+      </c>
+      <c r="N50" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E51" s="2">
+        <v>1.2509479999999999</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0.106195</v>
+      </c>
+      <c r="G51" s="2">
+        <v>14.347491</v>
+      </c>
+      <c r="H51" s="2">
+        <v>0.10000299999999999</v>
+      </c>
+      <c r="I51" s="2">
+        <v>5.6933999999999998E-2</v>
+      </c>
+      <c r="J51">
+        <v>45</v>
+      </c>
+      <c r="K51">
+        <v>200</v>
+      </c>
+      <c r="L51">
+        <v>100</v>
+      </c>
+      <c r="M51" t="s">
+        <v>37</v>
+      </c>
+      <c r="N51" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E52" s="2">
+        <v>1.233257</v>
+      </c>
+      <c r="F52" s="2">
+        <v>0.105693</v>
+      </c>
+      <c r="G52" s="2">
+        <v>14.464691</v>
+      </c>
+      <c r="H52" s="2">
+        <v>9.9141000000000007E-2</v>
+      </c>
+      <c r="I52" s="2">
+        <v>6.1615000000000003E-2</v>
+      </c>
+      <c r="J52">
+        <v>46</v>
+      </c>
+      <c r="K52">
+        <v>200</v>
+      </c>
+      <c r="L52">
+        <v>100</v>
+      </c>
+      <c r="M52" t="s">
+        <v>37</v>
+      </c>
+      <c r="N52" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E53" s="2">
+        <v>1.222467</v>
+      </c>
+      <c r="F53" s="2">
+        <v>0.105057</v>
+      </c>
+      <c r="G53" s="2">
+        <v>14.938568999999999</v>
+      </c>
+      <c r="H53" s="2">
+        <v>0.100059</v>
+      </c>
+      <c r="I53" s="2">
+        <v>6.1869E-2</v>
+      </c>
+      <c r="J53">
+        <v>47</v>
+      </c>
+      <c r="K53">
+        <v>200</v>
+      </c>
+      <c r="L53">
+        <v>100</v>
+      </c>
+      <c r="M53" t="s">
+        <v>37</v>
+      </c>
+      <c r="N53" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E54" s="2">
+        <v>1.2200949999999999</v>
+      </c>
+      <c r="F54" s="2">
+        <v>0.10652300000000001</v>
+      </c>
+      <c r="G54" s="2">
+        <v>15.547212</v>
+      </c>
+      <c r="H54" s="2">
+        <v>0.100422</v>
+      </c>
+      <c r="I54" s="2">
+        <v>6.1690000000000002E-2</v>
+      </c>
+      <c r="J54">
+        <v>48</v>
+      </c>
+      <c r="K54">
+        <v>200</v>
+      </c>
+      <c r="L54">
+        <v>100</v>
+      </c>
+      <c r="M54" t="s">
+        <v>37</v>
+      </c>
+      <c r="N54" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E55" s="2">
+        <v>1.1992750000000001</v>
+      </c>
+      <c r="F55" s="2">
+        <v>0.105235</v>
+      </c>
+      <c r="G55" s="2">
+        <v>13.041757</v>
+      </c>
+      <c r="H55" s="2">
+        <v>9.7867999999999997E-2</v>
+      </c>
+      <c r="I55" s="2">
+        <v>5.7001999999999997E-2</v>
+      </c>
+      <c r="J55">
+        <v>49</v>
+      </c>
+      <c r="K55">
+        <v>200</v>
+      </c>
+      <c r="L55">
+        <v>100</v>
+      </c>
+      <c r="M55" t="s">
+        <v>37</v>
+      </c>
+      <c r="N55" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E56" s="2">
+        <v>1.2529889999999999</v>
+      </c>
+      <c r="F56" s="2">
+        <v>0.107449</v>
+      </c>
+      <c r="G56" s="2">
+        <v>15.048621000000001</v>
+      </c>
+      <c r="H56" s="2">
+        <v>0.100561</v>
+      </c>
+      <c r="I56" s="2">
+        <v>6.0361999999999999E-2</v>
+      </c>
+      <c r="J56">
+        <v>50</v>
+      </c>
+      <c r="K56">
+        <v>200</v>
+      </c>
+      <c r="L56">
+        <v>100</v>
+      </c>
+      <c r="M56" t="s">
+        <v>37</v>
+      </c>
+      <c r="N56" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E57" s="2">
+        <v>1.235001</v>
+      </c>
+      <c r="F57" s="2">
+        <v>0.105688</v>
+      </c>
+      <c r="G57" s="2">
+        <v>11.637117</v>
+      </c>
+      <c r="H57" s="2">
+        <v>9.8295999999999994E-2</v>
+      </c>
+      <c r="I57" s="2">
+        <v>6.1691999999999997E-2</v>
+      </c>
+      <c r="J57">
+        <v>51</v>
+      </c>
+      <c r="K57">
+        <v>200</v>
+      </c>
+      <c r="L57">
+        <v>100</v>
+      </c>
+      <c r="M57" t="s">
+        <v>37</v>
+      </c>
+      <c r="N57" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>24000</v>
+      </c>
+      <c r="B61">
+        <v>6020</v>
+      </c>
+      <c r="C61" t="s">
+        <v>34</v>
+      </c>
+      <c r="J61">
+        <v>42</v>
+      </c>
+      <c r="K61">
+        <v>400</v>
+      </c>
+      <c r="L61">
+        <v>200</v>
+      </c>
+      <c r="M61" t="s">
+        <v>32</v>
+      </c>
+      <c r="N61" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J62">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J63">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J64">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="65" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J65">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="66" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J66">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="67" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J67">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="68" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J68">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="69" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J69">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="70" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J70">
         <v>51</v>
       </c>
     </row>

</xml_diff>